<commit_message>
refactored decision engine; made a new model based on random sampling of position data
</commit_message>
<xml_diff>
--- a/EngineInteraction.xlsx
+++ b/EngineInteraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\source\repos\AiChessEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87B09E86-64F4-450D-A1B5-AE8E92D46C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4799D98D-5A4A-41E6-AE4E-48A6F289915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48120" yWindow="795" windowWidth="20865" windowHeight="19350" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
+    <workbookView xWindow="48120" yWindow="795" windowWidth="25485" windowHeight="19350" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</t>
   </si>
@@ -45,25 +45,22 @@
     <t>" 0</t>
   </si>
   <si>
-    <t>5, 0, 0, 0, 0, 5, 9, 0,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1, 1, 8, 2, 0, 1, 1, 0,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, 1, 3, 1, 2, 0, 1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0,-1,-1, 0, 0, 0, 0,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -1,-1, 0, -3,-1,-1,-3,-1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, -2, 0, 0,-2,-1, 0,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -5, 0, 0,-8, 0,-5,-9, 0</t>
+    <t xml:space="preserve"> 1, 1, 1, 0, 1, 1, 1, 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</t>
+  </si>
+  <si>
+    <t>5, 2, 0, 8, 9, 3, 2, 5,</t>
+  </si>
+  <si>
+    <t>-1,-1,-1,-1,-1,-1,-1,-1,</t>
+  </si>
+  <si>
+    <t>-5, 0,-3,-8,-9,-3,-2,-5</t>
+  </si>
+  <si>
+    <t>-2, 0, 0, 0, 0, 0, 0, 0,</t>
   </si>
 </sst>
 </file>
@@ -418,84 +415,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179BEDD3-BBA2-415D-ACFC-FB77CC42443D}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="156.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="156.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A8</f>
+        <v>-5, 0,-3,-8,-9,-3,-2,-5</v>
+      </c>
+      <c r="E1" t="str">
+        <f>A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8</f>
+        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="str">
-        <f>A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8</f>
-        <v>5, 0, 0, 0, 0, 5, 9, 0, 1, 1, 8, 2, 0, 1, 1, 0, 0, 0, 1, 3, 1, 2, 0, 1, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0,-1,-1, 0, 0, 0, 0, 0, 0, -2, 0, 0,-2,-1, 0, -1,-1, 0, -3,-1,-1,-3,-1, -5, 0, 0,-8, 0,-5,-9, 0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="str">
+        <f>A7</f>
+        <v>-1,-1,-1,-1,-1,-1,-1,-1,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="str">
-        <f>_xlfn.VALUETOTEXT(C1)</f>
-        <v>5, 0, 0, 0, 0, 5, 9, 0, 1, 1, 8, 2, 0, 1, 1, 0, 0, 0, 1, 3, 1, 2, 0, 1, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0,-1,-1, 0, 0, 0, 0, 0, 0, -2, 0, 0,-2,-1, 0, -1,-1, 0, -3,-1,-1,-3,-1, -5, 0, 0,-8, 0,-5,-9, 0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>A6</f>
+        <v>-2, 0, 0, 0, 0, 0, 0, 0,</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xlfn.VALUETOTEXT(E1)</f>
+        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="str">
+        <f>A5</f>
+        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <f>A4</f>
+        <v xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="str">
+        <f>A3</f>
+        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <f>A2</f>
+        <v xml:space="preserve"> 1, 1, 1, 0, 1, 1, 1, 1,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
       <c r="C8" t="str">
-        <f>C5&amp;C3&amp;C6</f>
-        <v>./DecisionEngine.exe "5, 0, 0, 0, 0, 5, 9, 0, 1, 1, 8, 2, 0, 1, 1, 0, 0, 0, 1, 3, 1, 2, 0, 1, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0,-1,-1, 0, 0, 0, 0, 0, 0, -2, 0, 0,-2,-1, 0, -1,-1, 0, -3,-1,-1,-3,-1, -5, 0, 0,-8, 0,-5,-9, 0" 0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="str">
-        <f>_xlfn.VALUETOTEXT(C8)</f>
-        <v>./DecisionEngine.exe "5, 0, 0, 0, 0, 5, 9, 0, 1, 1, 8, 2, 0, 1, 1, 0, 0, 0, 1, 3, 1, 2, 0, 1, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0,-1,-1, 0, 0, 0, 0, 0, 0, -2, 0, 0,-2,-1, 0, -1,-1, 0, -3,-1,-1,-3,-1, -5, 0, 0,-8, 0,-5,-9, 0" 0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
+        <f>A1</f>
+        <v>5, 2, 0, 8, 9, 3, 2, 5,</v>
+      </c>
+      <c r="E8" t="str">
+        <f>E5&amp;E3&amp;E6</f>
+        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5" 0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
+        <f>_xlfn.VALUETOTEXT(E8)</f>
+        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5" 0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28">
         <v>4.5087903738021802E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more improvements to the decision engine; playing around with new model architectures
</commit_message>
<xml_diff>
--- a/EngineInteraction.xlsx
+++ b/EngineInteraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\source\repos\AiChessEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4799D98D-5A4A-41E6-AE4E-48A6F289915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB3C59D-5855-4290-88FF-A060B2AB4710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48120" yWindow="795" windowWidth="25485" windowHeight="19350" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
+    <workbookView xWindow="48120" yWindow="795" windowWidth="28515" windowHeight="19350" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,31 +36,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
-    <t xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</t>
-  </si>
-  <si>
     <t>./DecisionEngine.exe "</t>
   </si>
   <si>
     <t>" 0</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1, 1, 1, 0, 1, 1, 1, 1,</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</t>
   </si>
   <si>
-    <t>5, 2, 0, 8, 9, 3, 2, 5,</t>
-  </si>
-  <si>
-    <t>-1,-1,-1,-1,-1,-1,-1,-1,</t>
-  </si>
-  <si>
-    <t>-5, 0,-3,-8,-9,-3,-2,-5</t>
-  </si>
-  <si>
-    <t>-2, 0, 0, 0, 0, 0, 0, 0,</t>
+    <t>-1,-1,-1,-1, 0,-1,-1,-1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0, 1,-1, 0, 0, 0,</t>
+  </si>
+  <si>
+    <t>-5,-2,-3, 0,-9,-3,-2,-5</t>
+  </si>
+  <si>
+    <t>5, 2, 3, 8, 9, 3, 0, 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1, 1, 1, 0, 1, 1, 0, 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0, 0, 0, 2, 0, 1,</t>
   </si>
 </sst>
 </file>
@@ -430,46 +430,46 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" t="str">
         <f>A8</f>
-        <v>-5, 0,-3,-8,-9,-3,-2,-5</v>
+        <v>-5,-2,-3, 0,-9,-3,-2,-5</v>
       </c>
       <c r="E1" t="str">
         <f>A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8</f>
-        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5</v>
+        <v>5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C2" t="str">
         <f>A7</f>
-        <v>-1,-1,-1,-1,-1,-1,-1,-1,</v>
+        <v>-1,-1,-1,-1, 0,-1,-1,-1,</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" t="str">
         <f>A6</f>
-        <v>-2, 0, 0, 0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
       </c>
       <c r="E3" t="str">
         <f>_xlfn.VALUETOTEXT(E1)</f>
-        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5</v>
+        <v>5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f>A5</f>
-        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 0, 1,-1, 0, 0, 0,</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -478,50 +478,50 @@
       </c>
       <c r="C5" t="str">
         <f>A4</f>
-        <v xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" t="str">
         <f>A3</f>
-        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 0, 0, 0, 2, 0, 1,</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" t="str">
         <f>A2</f>
-        <v xml:space="preserve"> 1, 1, 1, 0, 1, 1, 1, 1,</v>
+        <v xml:space="preserve"> 1, 1, 1, 0, 1, 1, 0, 1,</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="str">
         <f>A1</f>
-        <v>5, 2, 0, 8, 9, 3, 2, 5,</v>
+        <v>5, 2, 3, 8, 9, 3, 0, 5,</v>
       </c>
       <c r="E8" t="str">
         <f>E5&amp;E3&amp;E6</f>
-        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5" 0</v>
+        <v>./DecisionEngine.exe "5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5" 0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E10" t="str">
         <f>_xlfn.VALUETOTEXT(E8)</f>
-        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-2, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1,-1,-1,-1,-1,-5, 0,-3,-8,-9,-3,-2,-5" 0</v>
+        <v>./DecisionEngine.exe "5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5" 0</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new models with much lower loss
</commit_message>
<xml_diff>
--- a/EngineInteraction.xlsx
+++ b/EngineInteraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\source\repos\AiChessEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrunaugh\source\repos\Personal\AiChessEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB3C59D-5855-4290-88FF-A060B2AB4710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1A6E77-69F4-44F3-AFD0-A219BC0E885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48120" yWindow="795" windowWidth="28515" windowHeight="19350" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>./DecisionEngine.exe "</t>
   </si>
@@ -42,25 +42,28 @@
     <t>" 0</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</t>
-  </si>
-  <si>
-    <t>-1,-1,-1,-1, 0,-1,-1,-1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, 0, 1,-1, 0, 0, 0,</t>
-  </si>
-  <si>
-    <t>-5,-2,-3, 0,-9,-3,-2,-5</t>
-  </si>
-  <si>
-    <t>5, 2, 3, 8, 9, 3, 0, 5,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1, 1, 1, 0, 1, 1, 0, 1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, 0, 0, 0, 2, 0, 1,</t>
+    <t xml:space="preserve"> 0, 0, 0,-1, 0, 0, 0, 0,</t>
+  </si>
+  <si>
+    <t>-1,-1,-1, 0,-1,-1,-1,-1,</t>
+  </si>
+  <si>
+    <t>5, 2, 0, 8, 9, 3, 2, 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -5, 0,-3,-8,-9,-3,-2,-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 2, 0, 0, 0, 0, 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1, 1, 1, 0, 0, 1, 1, 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0, 0, 1, 0, 0, 0,</t>
   </si>
 </sst>
 </file>
@@ -421,110 +424,110 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="156.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="156.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="str">
         <f>A8</f>
-        <v>-5,-2,-3, 0,-9,-3,-2,-5</v>
+        <v xml:space="preserve"> -5, 0,-3,-8,-9,-3,-2,-5</v>
       </c>
       <c r="E1" t="str">
         <f>A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8</f>
-        <v>5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="str">
         <f>A7</f>
-        <v>-1,-1,-1,-1, 0,-1,-1,-1,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1,-1,-1, 0,-1,-1,-1,-1,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="str">
         <f>A6</f>
-        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 2, 0, 0, 0, 0, 0,</v>
       </c>
       <c r="E3" t="str">
         <f>_xlfn.VALUETOTEXT(E1)</f>
-        <v>5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" t="str">
         <f>A5</f>
-        <v xml:space="preserve"> 0, 0, 0, 1,-1, 0, 0, 0,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> 0, 0, 0,-1, 0, 0, 0, 0,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="str">
         <f>A4</f>
-        <v xml:space="preserve"> 0, 0, 0, 0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6" t="str">
         <f>A3</f>
-        <v xml:space="preserve"> 0, 0, 0, 0, 0, 2, 0, 1,</v>
+        <v xml:space="preserve"> 0, 0, 0, 0, 1, 0, 0, 0,</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="str">
         <f>A2</f>
-        <v xml:space="preserve"> 1, 1, 1, 0, 1, 1, 0, 1,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> 1, 1, 1, 0, 0, 1, 1, 1,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="str">
         <f>A1</f>
-        <v>5, 2, 3, 8, 9, 3, 0, 5,</v>
+        <v>5, 2, 0, 8, 9, 3, 2, 5,</v>
       </c>
       <c r="E8" t="str">
         <f>E5&amp;E3&amp;E6</f>
-        <v>./DecisionEngine.exe "5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5" 0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5" 0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E10" t="str">
         <f>_xlfn.VALUETOTEXT(E8)</f>
-        <v>./DecisionEngine.exe "5, 2, 3, 8, 9, 3, 0, 5, 1, 1, 1, 0, 1, 1, 0, 1, 0, 0, 0, 0, 0, 2, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1,-1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1,-1,-1,-1, 0,-1,-1,-1,-5,-2,-3, 0,-9,-3,-2,-5" 0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5" 0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>4.5087903738021802E-2</v>
       </c>

</xml_diff>

<commit_message>
made a lot of progress on every component
</commit_message>
<xml_diff>
--- a/EngineInteraction.xlsx
+++ b/EngineInteraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrunaugh\source\repos\Personal\AiChessEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruna\source\repos\AiChessEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1A6E77-69F4-44F3-AFD0-A219BC0E885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDDF91A-068F-4858-BF0F-92F86866BEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
+    <workbookView xWindow="51690" yWindow="600" windowWidth="24435" windowHeight="19350" xr2:uid="{8DFA8606-8D6E-44DE-9D40-D9BFEC2E7FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,31 +39,31 @@
     <t>./DecisionEngine.exe "</t>
   </si>
   <si>
-    <t>" 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, 0,-1, 0, 0, 0, 0,</t>
-  </si>
-  <si>
-    <t>-1,-1,-1, 0,-1,-1,-1,-1,</t>
-  </si>
-  <si>
-    <t>5, 2, 0, 8, 9, 3, 2, 5,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -5, 0,-3,-8,-9,-3,-2,-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0, 0, 2, 0, 0, 0, 0, 0,</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1, 1, 1, 0, 0, 1, 1, 1,</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0, 0, 0, 0, 1, 0, 0, 0,</t>
+    <t>-5,-2,-3,-8,-9,-3,-2,-5</t>
+  </si>
+  <si>
+    <t>" 0 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,-1, 0, 1, 0, 3, 0, 0,</t>
+  </si>
+  <si>
+    <t>5, 2, 0, 8, 9, 0, 0, 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0, 3, 1, 2, 0, 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0,-1, 0, 0, 0,-1, 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0, 0, 0,-1,-1, 0, 0,-1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -1, 0, 0, 0, 0, 0, 0, 0,</t>
   </si>
 </sst>
 </file>
@@ -424,110 +424,110 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="156.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="156.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="str">
         <f>A8</f>
-        <v xml:space="preserve"> -5, 0,-3,-8,-9,-3,-2,-5</v>
+        <v>-5,-2,-3,-8,-9,-3,-2,-5</v>
       </c>
       <c r="E1" t="str">
         <f>A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8</f>
-        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5, 2, 0, 8, 9, 0, 0, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 3, 1, 2, 0, 0, 0,-1, 0, 1, 0, 3, 0, 0, -1, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1, 0, 0, 0,-1, 0, 0, 0, 0,-1,-1, 0, 0,-1,-5,-2,-3,-8,-9,-3,-2,-5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
         <f>A7</f>
-        <v>-1,-1,-1, 0,-1,-1,-1,-1,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v xml:space="preserve"> 0, 0, 0,-1,-1, 0, 0,-1,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="str">
         <f>A6</f>
-        <v xml:space="preserve"> 0, 0, 2, 0, 0, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0,-1, 0, 0, 0,-1, 0,</v>
       </c>
       <c r="E3" t="str">
         <f>_xlfn.VALUETOTEXT(E1)</f>
-        <v>5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5, 2, 0, 8, 9, 0, 0, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 3, 1, 2, 0, 0, 0,-1, 0, 1, 0, 3, 0, 0, -1, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1, 0, 0, 0,-1, 0, 0, 0, 0,-1,-1, 0, 0,-1,-5,-2,-3,-8,-9,-3,-2,-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="str">
         <f>A5</f>
-        <v xml:space="preserve"> 0, 0, 0,-1, 0, 0, 0, 0,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v xml:space="preserve"> -1, 0, 0, 0, 0, 0, 0, 0,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C5" t="str">
         <f>A4</f>
-        <v xml:space="preserve"> 0, 0, 0, 1, 0, 3, 0, 0,</v>
+        <v xml:space="preserve"> 0,-1, 0, 1, 0, 3, 0, 0,</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="str">
         <f>A3</f>
-        <v xml:space="preserve"> 0, 0, 0, 0, 1, 0, 0, 0,</v>
+        <v xml:space="preserve"> 0, 0, 0, 3, 1, 2, 0, 0,</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C7" t="str">
         <f>A2</f>
         <v xml:space="preserve"> 1, 1, 1, 0, 0, 1, 1, 1,</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C8" t="str">
         <f>A1</f>
-        <v>5, 2, 0, 8, 9, 3, 2, 5,</v>
+        <v>5, 2, 0, 8, 9, 0, 0, 5,</v>
       </c>
       <c r="E8" t="str">
         <f>E5&amp;E3&amp;E6</f>
-        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5" 0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 0, 0, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 3, 1, 2, 0, 0, 0,-1, 0, 1, 0, 3, 0, 0, -1, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1, 0, 0, 0,-1, 0, 0, 0, 0,-1,-1, 0, 0,-1,-5,-2,-3,-8,-9,-3,-2,-5" 0 1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E10" t="str">
         <f>_xlfn.VALUETOTEXT(E8)</f>
-        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 3, 2, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 3, 0, 0, 0, 0, 0,-1, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0,-1,-1,-1, 0,-1,-1,-1,-1, -5, 0,-3,-8,-9,-3,-2,-5" 0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+        <v>./DecisionEngine.exe "5, 2, 0, 8, 9, 0, 0, 5, 1, 1, 1, 0, 0, 1, 1, 1, 0, 0, 0, 3, 1, 2, 0, 0, 0,-1, 0, 1, 0, 3, 0, 0, -1, 0, 0, 0, 0, 0, 0, 0, 0, 0,-1, 0, 0, 0,-1, 0, 0, 0, 0,-1,-1, 0, 0,-1,-5,-2,-3,-8,-9,-3,-2,-5" 0 1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>4.5087903738021802E-2</v>
       </c>

</xml_diff>